<commit_message>
add one line to xlxs
</commit_message>
<xml_diff>
--- a/Manage_CE.xlsx
+++ b/Manage_CE.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>DW</t>
+  </si>
+  <si>
+    <t>Push to github</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1002,13 +1011,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="9.375"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1022,6 +1035,20 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>20220529</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>